<commit_message>
select data finish 🤯🤯🤯
</commit_message>
<xml_diff>
--- a/process_data/GPP_6210501001.xlsx
+++ b/process_data/GPP_6210501001.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pantchanit/Documents/final_stat_pant/process_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF58910-5991-0341-8477-C59B1EF23057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56443326-5D41-D147-83E8-534E6A04736A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="4540" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{2C66FAEA-E0CB-8549-8FB7-1B1C9698EE09}"/>
+    <workbookView xWindow="-37900" yWindow="5380" windowWidth="38400" windowHeight="20360" activeTab="3" xr2:uid="{2C66FAEA-E0CB-8549-8FB7-1B1C9698EE09}"/>
   </bookViews>
   <sheets>
     <sheet name="raw" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="70">
   <si>
     <t>GROSS PROVINCIAL PRODUCT AT CURRENT MARKET PRICES</t>
   </si>
@@ -243,6 +243,12 @@
   <si>
     <t>จำนวนนักท่องเที่ยวชาวต่างชาติ (คน)</t>
   </si>
+  <si>
+    <t>เนื้อที่สำหรับปลูกนาข้าว (ไร่)</t>
+  </si>
+  <si>
+    <t>เนื้อที่สำหรับปลูกพืชไร่ (ไร่)</t>
+  </si>
 </sst>
 </file>
 
@@ -376,7 +382,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -510,6 +516,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -517,7 +549,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
@@ -739,8 +771,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
@@ -6529,10 +6569,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB9047E-B268-2648-8545-D88A4802D6F0}">
-  <dimension ref="A1:AK29"/>
+  <dimension ref="A1:AK32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6541,7 +6581,10 @@
     <col min="6" max="6" width="29.33203125" customWidth="1"/>
     <col min="8" max="8" width="31.83203125" customWidth="1"/>
     <col min="17" max="17" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="36.33203125" customWidth="1"/>
+    <col min="22" max="22" width="23.1640625" customWidth="1"/>
+    <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="18.6640625" customWidth="1"/>
     <col min="25" max="25" width="12" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="21.1640625" customWidth="1"/>
@@ -6550,7 +6593,7 @@
     <col min="30" max="30" width="43.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="180" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" ht="140" x14ac:dyDescent="0.2">
       <c r="A1" s="66" t="s">
         <v>56</v>
       </c>
@@ -6636,10 +6679,10 @@
         <v>54</v>
       </c>
       <c r="AC1" s="61" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AD1" s="61" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AE1" s="61" t="s">
         <v>55</v>
@@ -8055,11 +8098,11 @@
       <c r="AB17" s="65">
         <v>2541350</v>
       </c>
-      <c r="AC17" s="77">
-        <v>695858</v>
-      </c>
-      <c r="AD17" s="75">
-        <v>10147</v>
+      <c r="AC17" s="79">
+        <v>1149975</v>
+      </c>
+      <c r="AD17" s="79">
+        <v>825214</v>
       </c>
       <c r="AE17" s="62"/>
       <c r="AF17" s="56">
@@ -8151,11 +8194,11 @@
       <c r="AB18" s="65">
         <v>2541569</v>
       </c>
-      <c r="AC18" s="77">
-        <v>333161</v>
-      </c>
-      <c r="AD18" s="75">
-        <v>4904</v>
+      <c r="AC18" s="79">
+        <v>1154555</v>
+      </c>
+      <c r="AD18" s="79">
+        <v>812779</v>
       </c>
       <c r="AE18" s="62">
         <v>26</v>
@@ -8247,11 +8290,11 @@
       <c r="AB19" s="65">
         <v>2196101</v>
       </c>
-      <c r="AC19" s="77">
-        <v>966110</v>
-      </c>
-      <c r="AD19" s="75">
-        <v>6619</v>
+      <c r="AC19" s="79">
+        <v>1153432</v>
+      </c>
+      <c r="AD19" s="79">
+        <v>812975</v>
       </c>
       <c r="AE19" s="62">
         <v>40</v>
@@ -8345,11 +8388,11 @@
       <c r="AB20" s="65">
         <v>2189464</v>
       </c>
-      <c r="AC20" s="77">
-        <v>1010038</v>
-      </c>
-      <c r="AD20" s="75">
-        <v>7369</v>
+      <c r="AC20" s="79">
+        <v>1153662</v>
+      </c>
+      <c r="AD20" s="79">
+        <v>812719</v>
       </c>
       <c r="AE20" s="62">
         <v>32</v>
@@ -8443,11 +8486,11 @@
       <c r="AB21" s="65">
         <v>2211616</v>
       </c>
-      <c r="AC21" s="77">
-        <v>1025505</v>
-      </c>
-      <c r="AD21" s="75">
-        <v>7016</v>
+      <c r="AC21" s="79">
+        <v>1154050</v>
+      </c>
+      <c r="AD21" s="79">
+        <v>812522</v>
       </c>
       <c r="AE21" s="62">
         <v>37</v>
@@ -8541,11 +8584,11 @@
       <c r="AB22" s="65">
         <v>2191974</v>
       </c>
-      <c r="AC22" s="77">
-        <v>1078379</v>
-      </c>
-      <c r="AD22" s="75">
-        <v>8049</v>
+      <c r="AC22" s="79">
+        <v>1133959</v>
+      </c>
+      <c r="AD22" s="79">
+        <v>813100</v>
       </c>
       <c r="AE22" s="62">
         <v>59</v>
@@ -8639,11 +8682,11 @@
       <c r="AB23" s="65">
         <v>2191454</v>
       </c>
-      <c r="AC23" s="77">
-        <v>1098904</v>
-      </c>
-      <c r="AD23" s="75">
-        <v>8415</v>
+      <c r="AC23" s="79">
+        <v>1133991</v>
+      </c>
+      <c r="AD23" s="79">
+        <v>812485</v>
       </c>
       <c r="AE23" s="62">
         <v>31</v>
@@ -8737,11 +8780,11 @@
       <c r="AB24" s="65">
         <v>2191311</v>
       </c>
-      <c r="AC24" s="77">
-        <v>1148049</v>
-      </c>
-      <c r="AD24" s="75">
-        <v>8962</v>
+      <c r="AC24" s="79">
+        <v>1133430</v>
+      </c>
+      <c r="AD24" s="79">
+        <v>813167</v>
       </c>
       <c r="AE24" s="62">
         <v>19</v>
@@ -8833,11 +8876,11 @@
       <c r="AB25" s="65">
         <v>2191867</v>
       </c>
-      <c r="AC25" s="77">
-        <v>1107250</v>
-      </c>
-      <c r="AD25" s="75">
-        <v>8501</v>
+      <c r="AC25" s="79">
+        <v>1134183</v>
+      </c>
+      <c r="AD25" s="79">
+        <v>812834</v>
       </c>
       <c r="AE25" s="62">
         <v>30</v>
@@ -8858,15 +8901,31 @@
       <c r="AK28" s="73"/>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="AC29" s="74"/>
-      <c r="AD29" s="74"/>
-      <c r="AE29" s="74"/>
-      <c r="AF29" s="74"/>
-      <c r="AG29" s="74"/>
+      <c r="X29" s="78"/>
+      <c r="Y29" s="78"/>
+      <c r="Z29" s="78"/>
+      <c r="AA29" s="78"/>
+      <c r="AB29" s="78"/>
+      <c r="AC29" s="78"/>
+      <c r="AD29" s="78"/>
+      <c r="AE29" s="78"/>
+      <c r="AF29" s="78"/>
+      <c r="AG29" s="77"/>
       <c r="AH29" s="74"/>
       <c r="AI29" s="74"/>
       <c r="AJ29" s="74"/>
       <c r="AK29" s="74"/>
+    </row>
+    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AA32" s="78"/>
+      <c r="AB32" s="78"/>
+      <c r="AC32" s="78"/>
+      <c r="AD32" s="78"/>
+      <c r="AE32" s="78"/>
+      <c r="AF32" s="78"/>
+      <c r="AG32" s="78"/>
+      <c r="AH32" s="78"/>
+      <c r="AI32" s="78"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8875,10 +8934,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B32E04E-C22B-ED4B-85C4-796A1BDA05F3}">
-  <dimension ref="A1:AF32"/>
+  <dimension ref="A1:AG32"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="U27" sqref="U27"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8890,7 +8949,8 @@
     <col min="23" max="23" width="26.6640625" customWidth="1"/>
     <col min="24" max="24" width="22.6640625" customWidth="1"/>
     <col min="25" max="26" width="28.5" customWidth="1"/>
-    <col min="29" max="30" width="10.83203125" customWidth="1"/>
+    <col min="29" max="29" width="33" customWidth="1"/>
+    <col min="30" max="30" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="180" x14ac:dyDescent="0.2">
@@ -8979,10 +9039,10 @@
         <v>54</v>
       </c>
       <c r="AC1" s="61" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AD1" s="61" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AE1" s="61" t="s">
         <v>55</v>
@@ -10315,7 +10375,7 @@
         <v>379657.777</v>
       </c>
     </row>
-    <row r="17" spans="1:32" ht="20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" ht="20" x14ac:dyDescent="0.25">
       <c r="A17" s="70" t="s">
         <v>19</v>
       </c>
@@ -10398,18 +10458,18 @@
       <c r="AB17" s="47">
         <v>449686</v>
       </c>
-      <c r="AC17" s="75">
-        <v>130915</v>
-      </c>
-      <c r="AD17" s="75">
-        <v>1266</v>
+      <c r="AC17" s="79">
+        <v>105867</v>
+      </c>
+      <c r="AD17" s="79">
+        <v>313067</v>
       </c>
       <c r="AE17" s="51"/>
       <c r="AF17" s="50">
         <v>427733.43600000005</v>
       </c>
     </row>
-    <row r="18" spans="1:32" ht="20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" ht="20" x14ac:dyDescent="0.25">
       <c r="A18" s="66" t="s">
         <v>20</v>
       </c>
@@ -10494,11 +10554,11 @@
       <c r="AB18" s="47">
         <v>449681</v>
       </c>
-      <c r="AC18" s="75">
-        <v>113017</v>
-      </c>
-      <c r="AD18" s="78">
-        <v>932</v>
+      <c r="AC18" s="79">
+        <v>111656</v>
+      </c>
+      <c r="AD18" s="79">
+        <v>344589</v>
       </c>
       <c r="AE18" s="52">
         <v>9</v>
@@ -10507,7 +10567,7 @@
         <v>365800.94500000001</v>
       </c>
     </row>
-    <row r="19" spans="1:32" ht="20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" ht="20" x14ac:dyDescent="0.25">
       <c r="A19" s="66" t="s">
         <v>21</v>
       </c>
@@ -10590,11 +10650,11 @@
       <c r="AB19" s="47">
         <v>492314</v>
       </c>
-      <c r="AC19" s="75">
-        <v>164531</v>
-      </c>
-      <c r="AD19" s="78">
-        <v>945</v>
+      <c r="AC19" s="79">
+        <v>112165</v>
+      </c>
+      <c r="AD19" s="79">
+        <v>345037</v>
       </c>
       <c r="AE19" s="52">
         <v>6</v>
@@ -10603,7 +10663,7 @@
         <v>378620.53700000001</v>
       </c>
     </row>
-    <row r="20" spans="1:32" ht="20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" ht="20" x14ac:dyDescent="0.25">
       <c r="A20" s="66" t="s">
         <v>22</v>
       </c>
@@ -10688,11 +10748,11 @@
       <c r="AB20" s="47">
         <v>491212</v>
       </c>
-      <c r="AC20" s="75">
-        <v>162999</v>
-      </c>
-      <c r="AD20" s="78">
-        <v>856</v>
+      <c r="AC20" s="79">
+        <v>112054</v>
+      </c>
+      <c r="AD20" s="79">
+        <v>345116</v>
       </c>
       <c r="AE20" s="52">
         <v>8</v>
@@ -10701,7 +10761,7 @@
         <v>461789.49600000004</v>
       </c>
     </row>
-    <row r="21" spans="1:32" ht="20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" ht="20" x14ac:dyDescent="0.25">
       <c r="A21" s="66" t="s">
         <v>23</v>
       </c>
@@ -10786,11 +10846,11 @@
       <c r="AB21" s="47">
         <v>491553</v>
       </c>
-      <c r="AC21" s="75">
-        <v>172139</v>
-      </c>
-      <c r="AD21" s="78">
-        <v>875</v>
+      <c r="AC21" s="79">
+        <v>111942</v>
+      </c>
+      <c r="AD21" s="79">
+        <v>345313</v>
       </c>
       <c r="AE21" s="52">
         <v>4</v>
@@ -10799,7 +10859,7 @@
         <v>417614.34099999996</v>
       </c>
     </row>
-    <row r="22" spans="1:32" ht="20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" ht="20" x14ac:dyDescent="0.25">
       <c r="A22" s="66" t="s">
         <v>24</v>
       </c>
@@ -10884,11 +10944,11 @@
       <c r="AB22" s="47">
         <v>491350</v>
       </c>
-      <c r="AC22" s="75">
-        <v>184089</v>
-      </c>
-      <c r="AD22" s="78">
-        <v>922</v>
+      <c r="AC22" s="79">
+        <v>111778</v>
+      </c>
+      <c r="AD22" s="79">
+        <v>345205</v>
       </c>
       <c r="AE22" s="52">
         <v>6</v>
@@ -10897,7 +10957,7 @@
         <v>468325.83400000003</v>
       </c>
     </row>
-    <row r="23" spans="1:32" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="66">
         <v>2016</v>
       </c>
@@ -10982,11 +11042,11 @@
       <c r="AB23" s="47">
         <v>491322</v>
       </c>
-      <c r="AC23" s="75">
-        <v>188910</v>
-      </c>
-      <c r="AD23" s="78">
-        <v>953</v>
+      <c r="AC23" s="79">
+        <v>111677</v>
+      </c>
+      <c r="AD23" s="79">
+        <v>345244</v>
       </c>
       <c r="AE23" s="52">
         <v>11</v>
@@ -10995,7 +11055,7 @@
         <v>444803.565</v>
       </c>
     </row>
-    <row r="24" spans="1:32" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="66">
         <v>2017</v>
       </c>
@@ -11080,11 +11140,11 @@
       <c r="AB24" s="47">
         <v>491855</v>
       </c>
-      <c r="AC24" s="75">
-        <v>197075</v>
-      </c>
-      <c r="AD24" s="75">
-        <v>1014</v>
+      <c r="AC24" s="79">
+        <v>112365</v>
+      </c>
+      <c r="AD24" s="79">
+        <v>345124</v>
       </c>
       <c r="AE24" s="52">
         <v>6</v>
@@ -11093,7 +11153,7 @@
         <v>449602.96699999995</v>
       </c>
     </row>
-    <row r="25" spans="1:32" ht="19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="66">
         <v>2018</v>
       </c>
@@ -11176,11 +11236,11 @@
       <c r="AB25" s="47">
         <v>492113</v>
       </c>
-      <c r="AC25" s="75">
-        <v>200403</v>
-      </c>
-      <c r="AD25" s="75">
-        <v>1061</v>
+      <c r="AC25" s="79">
+        <v>112314</v>
+      </c>
+      <c r="AD25" s="79">
+        <v>345409</v>
       </c>
       <c r="AE25" s="52">
         <v>5</v>
@@ -11189,7 +11249,7 @@
         <v>454952.54100000003</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A26" s="71"/>
       <c r="B26" s="71"/>
       <c r="C26" s="71"/>
@@ -11217,7 +11277,7 @@
       <c r="Y26" s="71"/>
       <c r="Z26" s="71"/>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A27" s="71"/>
       <c r="B27" s="71"/>
       <c r="C27" s="71"/>
@@ -11245,7 +11305,7 @@
       <c r="Y27" s="71"/>
       <c r="Z27" s="71"/>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A28" s="71"/>
       <c r="B28" s="71"/>
       <c r="C28" s="71"/>
@@ -11273,7 +11333,7 @@
       <c r="Y28" s="71"/>
       <c r="Z28" s="71"/>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A29" s="71"/>
       <c r="B29" s="71"/>
       <c r="C29" s="71"/>
@@ -11298,10 +11358,17 @@
       <c r="V29" s="71"/>
       <c r="W29" s="71"/>
       <c r="X29" s="71"/>
-      <c r="Y29" s="71"/>
-      <c r="Z29" s="71"/>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="Y29" s="78"/>
+      <c r="Z29" s="78"/>
+      <c r="AA29" s="78"/>
+      <c r="AB29" s="78"/>
+      <c r="AC29" s="78"/>
+      <c r="AD29" s="78"/>
+      <c r="AE29" s="78"/>
+      <c r="AF29" s="78"/>
+      <c r="AG29" s="78"/>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A30" s="71"/>
       <c r="B30" s="71"/>
       <c r="C30" s="71"/>
@@ -11325,16 +11392,18 @@
       <c r="U30" s="71"/>
       <c r="V30" s="71"/>
       <c r="W30" s="74"/>
-      <c r="X30" s="74"/>
-      <c r="Y30" s="74"/>
-      <c r="Z30" s="74"/>
-      <c r="AA30" s="74"/>
-      <c r="AB30" s="74"/>
-      <c r="AC30" s="74"/>
-      <c r="AD30" s="74"/>
-      <c r="AE30" s="74"/>
-    </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="X30" s="80"/>
+      <c r="Y30" s="78"/>
+      <c r="Z30" s="78"/>
+      <c r="AA30" s="78"/>
+      <c r="AB30" s="78"/>
+      <c r="AC30" s="78"/>
+      <c r="AD30" s="78"/>
+      <c r="AE30" s="78"/>
+      <c r="AF30" s="78"/>
+      <c r="AG30" s="78"/>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A31" s="71"/>
       <c r="B31" s="71"/>
       <c r="C31" s="71"/>
@@ -11362,7 +11431,7 @@
       <c r="Y31" s="71"/>
       <c r="Z31" s="71"/>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A32" s="71"/>
       <c r="B32" s="71"/>
       <c r="C32" s="71"/>

</xml_diff>

<commit_message>
change some factor 🥶
</commit_message>
<xml_diff>
--- a/process_data/GPP_6210501001.xlsx
+++ b/process_data/GPP_6210501001.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pantchanit/Documents/final_stat_pant/process_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F8FB17-4E2A-5346-A155-4D3E1F0DAD61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5119D877-AC04-4849-AEAC-6E38E4D98862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30880" yWindow="4540" windowWidth="38400" windowHeight="20360" xr2:uid="{2C66FAEA-E0CB-8549-8FB7-1B1C9698EE09}"/>
+    <workbookView xWindow="-33400" yWindow="4540" windowWidth="38400" windowHeight="20360" activeTab="3" xr2:uid="{2C66FAEA-E0CB-8549-8FB7-1B1C9698EE09}"/>
   </bookViews>
   <sheets>
     <sheet name="raw" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="68">
   <si>
     <t>GROSS PROVINCIAL PRODUCT AT CURRENT MARKET PRICES</t>
   </si>
@@ -238,16 +238,10 @@
     <t>ค่าใช้จ่ายในการวิจัยและพัฒนา (คิดเป็น % ของจีดีพี)</t>
   </si>
   <si>
-    <t>จำนวนนักท่องเที่ยวชาวไทย (คน)</t>
-  </si>
-  <si>
-    <t>จำนวนนักท่องเที่ยวชาวต่างชาติ (คน)</t>
-  </si>
-  <si>
     <t>เนื้อที่สำหรับปลูกนาข้าว (ไร่)</t>
   </si>
   <si>
-    <t>เนื้อที่สำหรับปลูกพืชไร่ (ไร่)</t>
+    <t>เนื้อที่สวนผักและไม้ดอก (ไร่)</t>
   </si>
 </sst>
 </file>
@@ -257,7 +251,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-1010409]#,##0;\-#,##0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -329,6 +323,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -549,7 +555,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
@@ -765,9 +771,6 @@
     <xf numFmtId="3" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -782,6 +785,18 @@
     </xf>
     <xf numFmtId="3" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1100,7 +1115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B33E03C5-685B-5940-859A-56FF0EBDBC17}">
   <dimension ref="A1:Y63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
@@ -4223,10 +4238,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244176B4-7511-5248-99A4-5973B793F41B}">
-  <dimension ref="A1:AQ25"/>
+  <dimension ref="A1:AQ29"/>
   <sheetViews>
     <sheetView topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+      <selection activeCell="AC1" sqref="AC1:AD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4334,10 +4349,10 @@
         <v>54</v>
       </c>
       <c r="AC1" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD1" s="61" t="s">
         <v>66</v>
-      </c>
-      <c r="AD1" s="61" t="s">
-        <v>67</v>
       </c>
       <c r="AE1" s="61" t="s">
         <v>55</v>
@@ -5688,7 +5703,7 @@
         <v>379657.777</v>
       </c>
     </row>
-    <row r="17" spans="1:32" ht="19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="53">
         <v>2010</v>
       </c>
@@ -5771,18 +5786,18 @@
       <c r="AB17" s="65">
         <v>1155861</v>
       </c>
-      <c r="AC17" s="75">
-        <v>1068404</v>
-      </c>
-      <c r="AD17" s="75">
-        <v>241583</v>
+      <c r="AC17" s="81">
+        <v>9042</v>
+      </c>
+      <c r="AD17" s="81">
+        <v>1046128</v>
       </c>
       <c r="AE17" s="64"/>
       <c r="AF17" s="56">
         <v>427733.43600000005</v>
       </c>
     </row>
-    <row r="18" spans="1:32" ht="19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="53">
         <v>2011</v>
       </c>
@@ -5867,11 +5882,11 @@
       <c r="AB18" s="65">
         <v>1158113</v>
       </c>
-      <c r="AC18" s="75">
-        <v>851323</v>
-      </c>
-      <c r="AD18" s="75">
-        <v>176974</v>
+      <c r="AC18" s="81">
+        <v>9461</v>
+      </c>
+      <c r="AD18" s="81">
+        <v>1065030</v>
       </c>
       <c r="AE18" s="62">
         <v>147</v>
@@ -5880,7 +5895,7 @@
         <v>365800.94500000001</v>
       </c>
     </row>
-    <row r="19" spans="1:32" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="53">
         <v>2012</v>
       </c>
@@ -5963,11 +5978,11 @@
       <c r="AB19" s="65">
         <v>1180726</v>
       </c>
-      <c r="AC19" s="75">
-        <v>1068100</v>
-      </c>
-      <c r="AD19" s="75">
-        <v>319872</v>
+      <c r="AC19" s="81">
+        <v>9598</v>
+      </c>
+      <c r="AD19" s="81">
+        <v>1065565</v>
       </c>
       <c r="AE19" s="62">
         <v>109</v>
@@ -5976,7 +5991,7 @@
         <v>378620.53700000001</v>
       </c>
     </row>
-    <row r="20" spans="1:32" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="53">
         <v>2013</v>
       </c>
@@ -6061,11 +6076,11 @@
       <c r="AB20" s="65">
         <v>1177369</v>
       </c>
-      <c r="AC20" s="75">
-        <v>1073412</v>
-      </c>
-      <c r="AD20" s="75">
-        <v>319845</v>
+      <c r="AC20" s="81">
+        <v>9573.8304647791701</v>
+      </c>
+      <c r="AD20" s="81">
+        <v>1065335.81531144</v>
       </c>
       <c r="AE20" s="62">
         <v>93</v>
@@ -6074,7 +6089,7 @@
         <v>461789.49600000004</v>
       </c>
     </row>
-    <row r="21" spans="1:32" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="53">
         <v>2014</v>
       </c>
@@ -6159,11 +6174,11 @@
       <c r="AB21" s="65">
         <v>1178443</v>
       </c>
-      <c r="AC21" s="75">
-        <v>1142119</v>
-      </c>
-      <c r="AD21" s="75">
-        <v>343339</v>
+      <c r="AC21" s="81">
+        <v>9510</v>
+      </c>
+      <c r="AD21" s="81">
+        <v>1065583</v>
       </c>
       <c r="AE21" s="62">
         <v>117</v>
@@ -6172,7 +6187,7 @@
         <v>417614.34099999996</v>
       </c>
     </row>
-    <row r="22" spans="1:32" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="53">
         <v>2015</v>
       </c>
@@ -6257,11 +6272,11 @@
       <c r="AB22" s="65">
         <v>1177896</v>
       </c>
-      <c r="AC22" s="75">
-        <v>1205428</v>
-      </c>
-      <c r="AD22" s="75">
-        <v>343180</v>
+      <c r="AC22" s="81">
+        <v>9500</v>
+      </c>
+      <c r="AD22" s="81">
+        <v>1065016</v>
       </c>
       <c r="AE22" s="62">
         <v>132</v>
@@ -6270,7 +6285,7 @@
         <v>468325.83400000003</v>
       </c>
     </row>
-    <row r="23" spans="1:32" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="53">
         <v>2016</v>
       </c>
@@ -6355,11 +6370,11 @@
       <c r="AB23" s="65">
         <v>1178345</v>
       </c>
-      <c r="AC23" s="75">
-        <v>1237790</v>
-      </c>
-      <c r="AD23" s="75">
-        <v>345115</v>
+      <c r="AC23" s="81">
+        <v>9711</v>
+      </c>
+      <c r="AD23" s="81">
+        <v>1065315</v>
       </c>
       <c r="AE23" s="62">
         <v>121</v>
@@ -6368,7 +6383,7 @@
         <v>444803.565</v>
       </c>
     </row>
-    <row r="24" spans="1:32" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="53">
         <v>2017</v>
       </c>
@@ -6453,11 +6468,11 @@
       <c r="AB24" s="65">
         <v>1178698</v>
       </c>
-      <c r="AC24" s="75">
-        <v>1281574</v>
-      </c>
-      <c r="AD24" s="75">
-        <v>355607</v>
+      <c r="AC24" s="81">
+        <v>9720</v>
+      </c>
+      <c r="AD24" s="81">
+        <v>1065376</v>
       </c>
       <c r="AE24" s="62">
         <v>117</v>
@@ -6466,7 +6481,7 @@
         <v>449602.96699999995</v>
       </c>
     </row>
-    <row r="25" spans="1:32" ht="19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="53">
         <v>2018</v>
       </c>
@@ -6549,11 +6564,11 @@
       <c r="AB25" s="65">
         <v>1178475</v>
       </c>
-      <c r="AC25" s="75">
-        <v>1354163</v>
-      </c>
-      <c r="AD25" s="75">
-        <v>369547</v>
+      <c r="AC25" s="81">
+        <v>9713</v>
+      </c>
+      <c r="AD25" s="81">
+        <v>1065197</v>
       </c>
       <c r="AE25" s="62">
         <v>96</v>
@@ -6561,6 +6576,17 @@
       <c r="AF25" s="55">
         <v>454952.54100000003</v>
       </c>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AB29" s="82"/>
+      <c r="AC29" s="82"/>
+      <c r="AD29" s="82"/>
+      <c r="AE29" s="82"/>
+      <c r="AF29" s="82"/>
+      <c r="AG29" s="82"/>
+      <c r="AH29" s="82"/>
+      <c r="AI29" s="82"/>
+      <c r="AJ29" s="82"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6572,7 +6598,7 @@
   <dimension ref="A1:AK32"/>
   <sheetViews>
     <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AD1" sqref="AD1"/>
+      <selection activeCell="AC1" sqref="AC1:AC25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6679,10 +6705,10 @@
         <v>54</v>
       </c>
       <c r="AC1" s="61" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AD1" s="61" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AE1" s="61" t="s">
         <v>55</v>
@@ -8098,10 +8124,10 @@
       <c r="AB17" s="65">
         <v>2541350</v>
       </c>
-      <c r="AC17" s="79">
-        <v>1149975</v>
-      </c>
-      <c r="AD17" s="79">
+      <c r="AC17" s="81">
+        <v>20343</v>
+      </c>
+      <c r="AD17" s="78">
         <v>825214</v>
       </c>
       <c r="AE17" s="62"/>
@@ -8194,10 +8220,10 @@
       <c r="AB18" s="65">
         <v>2541569</v>
       </c>
-      <c r="AC18" s="79">
-        <v>1154555</v>
-      </c>
-      <c r="AD18" s="79">
+      <c r="AC18" s="81">
+        <v>20535</v>
+      </c>
+      <c r="AD18" s="78">
         <v>812779</v>
       </c>
       <c r="AE18" s="62">
@@ -8290,10 +8316,10 @@
       <c r="AB19" s="65">
         <v>2196101</v>
       </c>
-      <c r="AC19" s="79">
-        <v>1153432</v>
-      </c>
-      <c r="AD19" s="79">
+      <c r="AC19" s="81">
+        <v>20364</v>
+      </c>
+      <c r="AD19" s="78">
         <v>812975</v>
       </c>
       <c r="AE19" s="62">
@@ -8388,10 +8414,10 @@
       <c r="AB20" s="65">
         <v>2189464</v>
       </c>
-      <c r="AC20" s="79">
-        <v>1153662</v>
-      </c>
-      <c r="AD20" s="79">
+      <c r="AC20" s="81">
+        <v>20318.469064254801</v>
+      </c>
+      <c r="AD20" s="78">
         <v>812719</v>
       </c>
       <c r="AE20" s="62">
@@ -8486,10 +8512,10 @@
       <c r="AB21" s="65">
         <v>2211616</v>
       </c>
-      <c r="AC21" s="79">
-        <v>1154050</v>
-      </c>
-      <c r="AD21" s="79">
+      <c r="AC21" s="81">
+        <v>20634</v>
+      </c>
+      <c r="AD21" s="78">
         <v>812522</v>
       </c>
       <c r="AE21" s="62">
@@ -8584,10 +8610,10 @@
       <c r="AB22" s="65">
         <v>2191974</v>
       </c>
-      <c r="AC22" s="79">
-        <v>1133959</v>
-      </c>
-      <c r="AD22" s="79">
+      <c r="AC22" s="81">
+        <v>20630</v>
+      </c>
+      <c r="AD22" s="78">
         <v>813100</v>
       </c>
       <c r="AE22" s="62">
@@ -8682,10 +8708,10 @@
       <c r="AB23" s="65">
         <v>2191454</v>
       </c>
-      <c r="AC23" s="79">
-        <v>1133991</v>
-      </c>
-      <c r="AD23" s="79">
+      <c r="AC23" s="81">
+        <v>20629</v>
+      </c>
+      <c r="AD23" s="78">
         <v>812485</v>
       </c>
       <c r="AE23" s="62">
@@ -8780,10 +8806,10 @@
       <c r="AB24" s="65">
         <v>2191311</v>
       </c>
-      <c r="AC24" s="79">
-        <v>1133430</v>
-      </c>
-      <c r="AD24" s="79">
+      <c r="AC24" s="81">
+        <v>20523</v>
+      </c>
+      <c r="AD24" s="78">
         <v>813167</v>
       </c>
       <c r="AE24" s="62">
@@ -8876,10 +8902,10 @@
       <c r="AB25" s="65">
         <v>2191867</v>
       </c>
-      <c r="AC25" s="79">
-        <v>1134183</v>
-      </c>
-      <c r="AD25" s="79">
+      <c r="AC25" s="81">
+        <v>20527</v>
+      </c>
+      <c r="AD25" s="78">
         <v>812834</v>
       </c>
       <c r="AE25" s="62">
@@ -8901,31 +8927,42 @@
       <c r="AK28" s="73"/>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="X29" s="78"/>
-      <c r="Y29" s="78"/>
-      <c r="Z29" s="78"/>
-      <c r="AA29" s="78"/>
-      <c r="AB29" s="78"/>
-      <c r="AC29" s="78"/>
-      <c r="AD29" s="78"/>
-      <c r="AE29" s="78"/>
-      <c r="AF29" s="78"/>
-      <c r="AG29" s="77"/>
+      <c r="X29" s="77"/>
+      <c r="Y29" s="77"/>
+      <c r="Z29" s="77"/>
+      <c r="AA29" s="77"/>
+      <c r="AB29" s="77"/>
+      <c r="AC29" s="77"/>
+      <c r="AD29" s="77"/>
+      <c r="AE29" s="77"/>
+      <c r="AF29" s="77"/>
+      <c r="AG29" s="76"/>
       <c r="AH29" s="74"/>
       <c r="AI29" s="74"/>
       <c r="AJ29" s="74"/>
       <c r="AK29" s="74"/>
     </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AA30" s="80"/>
+      <c r="AB30" s="80"/>
+      <c r="AC30" s="80"/>
+      <c r="AD30" s="80"/>
+      <c r="AE30" s="80"/>
+      <c r="AF30" s="80"/>
+      <c r="AG30" s="80"/>
+      <c r="AH30" s="80"/>
+      <c r="AI30" s="80"/>
+    </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="AA32" s="78"/>
-      <c r="AB32" s="78"/>
-      <c r="AC32" s="78"/>
-      <c r="AD32" s="78"/>
-      <c r="AE32" s="78"/>
-      <c r="AF32" s="78"/>
-      <c r="AG32" s="78"/>
-      <c r="AH32" s="78"/>
-      <c r="AI32" s="78"/>
+      <c r="AA32" s="77"/>
+      <c r="AB32" s="77"/>
+      <c r="AC32" s="77"/>
+      <c r="AD32" s="77"/>
+      <c r="AE32" s="77"/>
+      <c r="AF32" s="77"/>
+      <c r="AG32" s="77"/>
+      <c r="AH32" s="77"/>
+      <c r="AI32" s="77"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8936,8 +8973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B32E04E-C22B-ED4B-85C4-796A1BDA05F3}">
   <dimension ref="A1:AG32"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AD1" sqref="AD1"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AC17" sqref="AC17:AC25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9039,10 +9076,10 @@
         <v>54</v>
       </c>
       <c r="AC1" s="61" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AD1" s="61" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AE1" s="61" t="s">
         <v>55</v>
@@ -10458,10 +10495,10 @@
       <c r="AB17" s="47">
         <v>449686</v>
       </c>
-      <c r="AC17" s="79">
-        <v>105867</v>
-      </c>
-      <c r="AD17" s="79">
+      <c r="AC17" s="83">
+        <v>2268</v>
+      </c>
+      <c r="AD17" s="78">
         <v>313067</v>
       </c>
       <c r="AE17" s="51"/>
@@ -10554,10 +10591,10 @@
       <c r="AB18" s="47">
         <v>449681</v>
       </c>
-      <c r="AC18" s="79">
-        <v>111656</v>
-      </c>
-      <c r="AD18" s="79">
+      <c r="AC18" s="83">
+        <v>2284</v>
+      </c>
+      <c r="AD18" s="78">
         <v>344589</v>
       </c>
       <c r="AE18" s="52">
@@ -10650,10 +10687,10 @@
       <c r="AB19" s="47">
         <v>492314</v>
       </c>
-      <c r="AC19" s="79">
-        <v>112165</v>
-      </c>
-      <c r="AD19" s="79">
+      <c r="AC19" s="83">
+        <v>2261</v>
+      </c>
+      <c r="AD19" s="78">
         <v>345037</v>
       </c>
       <c r="AE19" s="52">
@@ -10748,10 +10785,10 @@
       <c r="AB20" s="47">
         <v>491212</v>
       </c>
-      <c r="AC20" s="79">
-        <v>112054</v>
-      </c>
-      <c r="AD20" s="79">
+      <c r="AC20" s="83">
+        <v>2261.3418506463099</v>
+      </c>
+      <c r="AD20" s="78">
         <v>345116</v>
       </c>
       <c r="AE20" s="52">
@@ -10846,10 +10883,10 @@
       <c r="AB21" s="47">
         <v>491553</v>
       </c>
-      <c r="AC21" s="79">
-        <v>111942</v>
-      </c>
-      <c r="AD21" s="79">
+      <c r="AC21" s="83">
+        <v>2241</v>
+      </c>
+      <c r="AD21" s="78">
         <v>345313</v>
       </c>
       <c r="AE21" s="52">
@@ -10944,10 +10981,10 @@
       <c r="AB22" s="47">
         <v>491350</v>
       </c>
-      <c r="AC22" s="79">
-        <v>111778</v>
-      </c>
-      <c r="AD22" s="79">
+      <c r="AC22" s="83">
+        <v>2353</v>
+      </c>
+      <c r="AD22" s="78">
         <v>345205</v>
       </c>
       <c r="AE22" s="52">
@@ -11042,10 +11079,10 @@
       <c r="AB23" s="47">
         <v>491322</v>
       </c>
-      <c r="AC23" s="79">
-        <v>111677</v>
-      </c>
-      <c r="AD23" s="79">
+      <c r="AC23" s="83">
+        <v>2348</v>
+      </c>
+      <c r="AD23" s="78">
         <v>345244</v>
       </c>
       <c r="AE23" s="52">
@@ -11140,10 +11177,10 @@
       <c r="AB24" s="47">
         <v>491855</v>
       </c>
-      <c r="AC24" s="79">
-        <v>112365</v>
-      </c>
-      <c r="AD24" s="79">
+      <c r="AC24" s="83">
+        <v>2346</v>
+      </c>
+      <c r="AD24" s="78">
         <v>345124</v>
       </c>
       <c r="AE24" s="52">
@@ -11236,10 +11273,10 @@
       <c r="AB25" s="47">
         <v>492113</v>
       </c>
-      <c r="AC25" s="79">
-        <v>112314</v>
-      </c>
-      <c r="AD25" s="79">
+      <c r="AC25" s="83">
+        <v>2344</v>
+      </c>
+      <c r="AD25" s="78">
         <v>345409</v>
       </c>
       <c r="AE25" s="52">
@@ -11358,15 +11395,15 @@
       <c r="V29" s="71"/>
       <c r="W29" s="71"/>
       <c r="X29" s="71"/>
-      <c r="Y29" s="78"/>
-      <c r="Z29" s="78"/>
-      <c r="AA29" s="78"/>
-      <c r="AB29" s="78"/>
-      <c r="AC29" s="78"/>
-      <c r="AD29" s="78"/>
-      <c r="AE29" s="78"/>
-      <c r="AF29" s="78"/>
-      <c r="AG29" s="78"/>
+      <c r="Y29" s="77"/>
+      <c r="Z29" s="77"/>
+      <c r="AA29" s="77"/>
+      <c r="AB29" s="77"/>
+      <c r="AC29" s="77"/>
+      <c r="AD29" s="77"/>
+      <c r="AE29" s="77"/>
+      <c r="AF29" s="77"/>
+      <c r="AG29" s="77"/>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A30" s="71"/>
@@ -11392,16 +11429,16 @@
       <c r="U30" s="71"/>
       <c r="V30" s="71"/>
       <c r="W30" s="74"/>
-      <c r="X30" s="80"/>
-      <c r="Y30" s="78"/>
-      <c r="Z30" s="78"/>
-      <c r="AA30" s="78"/>
-      <c r="AB30" s="78"/>
-      <c r="AC30" s="78"/>
-      <c r="AD30" s="78"/>
-      <c r="AE30" s="78"/>
-      <c r="AF30" s="78"/>
-      <c r="AG30" s="78"/>
+      <c r="X30" s="79"/>
+      <c r="Y30" s="77"/>
+      <c r="Z30" s="77"/>
+      <c r="AA30" s="77"/>
+      <c r="AB30" s="77"/>
+      <c r="AC30" s="77"/>
+      <c r="AD30" s="77"/>
+      <c r="AE30" s="77"/>
+      <c r="AF30" s="77"/>
+      <c r="AG30" s="77"/>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A31" s="71"/>
@@ -11455,12 +11492,12 @@
       <c r="U32" s="71"/>
       <c r="V32" s="71"/>
       <c r="W32" s="74"/>
-      <c r="X32" s="76"/>
-      <c r="Y32" s="76"/>
-      <c r="Z32" s="76"/>
-      <c r="AA32" s="76"/>
-      <c r="AB32" s="76"/>
-      <c r="AC32" s="76"/>
+      <c r="X32" s="75"/>
+      <c r="Y32" s="75"/>
+      <c r="Z32" s="75"/>
+      <c r="AA32" s="75"/>
+      <c r="AB32" s="75"/>
+      <c r="AC32" s="75"/>
       <c r="AD32" s="74"/>
       <c r="AE32" s="74"/>
     </row>

</xml_diff>